<commit_message>
up to date gemaakt voor volgende volgende update
</commit_message>
<xml_diff>
--- a/xlsx/input-output-vars-v16a.xlsx
+++ b/xlsx/input-output-vars-v16a.xlsx
@@ -1,22 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdijkstra/Dropbox/cpb/git/saffier/v4-quarter-data/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdijkstra/Dropbox/cpb/git/saffier/v5-text/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74778D5-721D-8746-9273-3D59122BB453}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDB5BF3-4CFF-ED41-96CD-E03DB9BC48D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="23500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="21" r:id="rId1"/>
     <sheet name="output" sheetId="20" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -559,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1439D50-1B93-CA4B-A2EE-FA5B38E7B869}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="160" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -590,7 +602,7 @@
         <v>29</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -607,7 +619,7 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
@@ -621,7 +633,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
@@ -635,7 +647,7 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
@@ -649,7 +661,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
@@ -663,7 +675,7 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
@@ -677,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -689,7 +701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>

</xml_diff>